<commit_message>
Updated schema v1.7. Changed lower boundary for p-value.
</commit_message>
<xml_diff>
--- a/schema_definitions/template_schema_v1.7.xlsx
+++ b/schema_definitions/template_schema_v1.7.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tudorgroza/Desktop/_GARETH_/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tudorgroza/Work/EBI/IMPORT_TEST/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E4B8A8-EA48-CF40-A625-1BA110726D0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{062E95B9-B6A8-0C45-9183-11CED083FD03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38360" windowHeight="17540" activeTab="1" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="187">
   <si>
     <t>NAME</t>
   </si>
@@ -596,6 +596,9 @@
   </si>
   <si>
     <t>$p-value$</t>
+  </si>
+  <si>
+    <t>1|-5</t>
   </si>
 </sst>
 </file>
@@ -1943,7 +1946,7 @@
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2165,8 +2168,8 @@
       <c r="J5" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="L5" s="13">
-        <v>-5</v>
+      <c r="L5" s="13" t="s">
+        <v>186</v>
       </c>
       <c r="M5" s="13"/>
       <c r="N5" s="5" t="s">

</xml_diff>